<commit_message>
not sure about the year, looks like It's learning data
</commit_message>
<xml_diff>
--- a/adm/03_Feb_15_15_Grades-5100-B1-2E16;Programmering_og_problemløsning.xlsx
+++ b/adm/03_Feb_15_15_Grades-5100-B1-2E16;Programmering_og_problemløsning.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sporring/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sporring/repositories/PoP/adm/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="30560" yWindow="1460" windowWidth="31740" windowHeight="16800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="31740" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_03_Feb_15_15_Grades_5100_B1_2E16_Programmering_og_problemløsning" localSheetId="0">Sheet1!$A$1:$R$233</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -32,7 +32,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="03_Feb_15_15_Grades-5100-B1-2E16;Programmering_og_problemløsning" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/sporring/Downloads/03_Feb_15_15_Grades-5100-B1-2E16;Programmering_og_problemløsning.csv" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/sporring/Downloads/03_Feb_15_15_Grades-5100-B1-2E16;Programmering_og_problemløsning.csv" comma="1">
       <textFields count="42">
         <textField/>
         <textField/>
@@ -1919,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
-      <selection activeCell="A249" sqref="A249"/>
+    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
+      <selection activeCell="A234" sqref="A234:R249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2058,7 +2058,7 @@
         <v>20</v>
       </c>
       <c r="F3">
-        <f>SUM(G3:R3)</f>
+        <f t="shared" ref="F3:F66" si="1">SUM(G3:R3)</f>
         <v>11</v>
       </c>
       <c r="G3">
@@ -2112,7 +2112,7 @@
         <v>23</v>
       </c>
       <c r="F4">
-        <f>SUM(G4:R4)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G4">
@@ -2169,7 +2169,7 @@
         <v>2</v>
       </c>
       <c r="F5">
-        <f>SUM(G5:R5)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="G5">
@@ -2199,7 +2199,7 @@
         <v>28</v>
       </c>
       <c r="F6">
-        <f>SUM(G6:R6)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G6">
@@ -2253,7 +2253,7 @@
         <v>31</v>
       </c>
       <c r="F7">
-        <f>SUM(G7:R7)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G7">
@@ -2310,7 +2310,7 @@
         <v>8</v>
       </c>
       <c r="F8">
-        <f>SUM(G8:R8)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="G8">
@@ -2340,7 +2340,7 @@
         <v>31</v>
       </c>
       <c r="F9">
-        <f>SUM(G9:R9)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G9">
@@ -2394,7 +2394,7 @@
         <v>38</v>
       </c>
       <c r="F10">
-        <f>SUM(G10:R10)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G10">
@@ -2448,7 +2448,7 @@
         <v>31</v>
       </c>
       <c r="F11">
-        <f>SUM(G11:R11)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G11">
@@ -2502,7 +2502,7 @@
         <v>43</v>
       </c>
       <c r="F12">
-        <f>SUM(G12:R12)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G12">
@@ -2550,7 +2550,7 @@
         <v>46</v>
       </c>
       <c r="F13">
-        <f>SUM(G13:R13)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G13">
@@ -2604,7 +2604,7 @@
         <v>49</v>
       </c>
       <c r="F14">
-        <f>SUM(G14:R14)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G14">
@@ -2658,7 +2658,7 @@
         <v>23</v>
       </c>
       <c r="F15">
-        <f>SUM(G15:R15)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G15">
@@ -2712,7 +2712,7 @@
         <v>31</v>
       </c>
       <c r="F16">
-        <f>SUM(G16:R16)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G16">
@@ -2769,7 +2769,7 @@
         <v>56</v>
       </c>
       <c r="F17">
-        <f>SUM(G17:R17)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G17">
@@ -2823,7 +2823,7 @@
         <v>28</v>
       </c>
       <c r="F18">
-        <f>SUM(G18:R18)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G18">
@@ -2877,7 +2877,7 @@
         <v>20</v>
       </c>
       <c r="F19">
-        <f>SUM(G19:R19)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G19">
@@ -2934,7 +2934,7 @@
         <v>31</v>
       </c>
       <c r="F20">
-        <f>SUM(G20:R20)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G20">
@@ -2988,7 +2988,7 @@
         <v>28</v>
       </c>
       <c r="F21">
-        <f>SUM(G21:R21)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G21">
@@ -3042,7 +3042,7 @@
         <v>49</v>
       </c>
       <c r="F22">
-        <f>SUM(G22:R22)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G22">
@@ -3096,7 +3096,7 @@
         <v>28</v>
       </c>
       <c r="F23">
-        <f>SUM(G23:R23)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G23">
@@ -3150,7 +3150,7 @@
         <v>10</v>
       </c>
       <c r="F24">
-        <f>SUM(G24:R24)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="G24">
@@ -3180,7 +3180,7 @@
         <v>43</v>
       </c>
       <c r="F25">
-        <f>SUM(G25:R25)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G25">
@@ -3234,7 +3234,7 @@
         <v>28</v>
       </c>
       <c r="F26">
-        <f>SUM(G26:R26)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G26">
@@ -3291,7 +3291,7 @@
         <v>28</v>
       </c>
       <c r="F27">
-        <f>SUM(G27:R27)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="G27">
@@ -3330,7 +3330,7 @@
         <v>4</v>
       </c>
       <c r="F28">
-        <f>SUM(G28:R28)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G28">
@@ -3354,7 +3354,7 @@
         <v>49</v>
       </c>
       <c r="F29">
-        <f>SUM(G29:R29)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G29">
@@ -3411,7 +3411,7 @@
         <v>46</v>
       </c>
       <c r="F30">
-        <f>SUM(G30:R30)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G30">
@@ -3465,7 +3465,7 @@
         <v>28</v>
       </c>
       <c r="F31">
-        <f>SUM(G31:R31)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G31">
@@ -3519,7 +3519,7 @@
         <v>28</v>
       </c>
       <c r="F32">
-        <f>SUM(G32:R32)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G32">
@@ -3576,7 +3576,7 @@
         <v>46</v>
       </c>
       <c r="F33" s="2">
-        <f>SUM(G33:R33)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G33">
@@ -3630,7 +3630,7 @@
         <v>28</v>
       </c>
       <c r="F34">
-        <f>SUM(G34:R34)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G34">
@@ -3684,7 +3684,7 @@
         <v>49</v>
       </c>
       <c r="F35">
-        <f>SUM(G35:R35)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G35">
@@ -3738,7 +3738,7 @@
         <v>23</v>
       </c>
       <c r="F36">
-        <f>SUM(G36:R36)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="G36">
@@ -3783,7 +3783,7 @@
         <v>31</v>
       </c>
       <c r="F37">
-        <f>SUM(G37:R37)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G37">
@@ -3837,7 +3837,7 @@
         <v>28</v>
       </c>
       <c r="F38">
-        <f>SUM(G38:R38)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G38">
@@ -3894,7 +3894,7 @@
         <v>101</v>
       </c>
       <c r="F39">
-        <f>SUM(G39:R39)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G39">
@@ -3948,7 +3948,7 @@
         <v>49</v>
       </c>
       <c r="F40">
-        <f>SUM(G40:R40)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G40">
@@ -4002,7 +4002,7 @@
         <v>23</v>
       </c>
       <c r="F41">
-        <f>SUM(G41:R41)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G41">
@@ -4056,7 +4056,7 @@
         <v>23</v>
       </c>
       <c r="F42">
-        <f>SUM(G42:R42)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G42">
@@ -4113,7 +4113,7 @@
         <v>20</v>
       </c>
       <c r="F43">
-        <f>SUM(G43:R43)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G43">
@@ -4167,7 +4167,7 @@
         <v>28</v>
       </c>
       <c r="F44">
-        <f>SUM(G44:R44)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G44">
@@ -4224,7 +4224,7 @@
         <v>56</v>
       </c>
       <c r="F45">
-        <f>SUM(G45:R45)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G45">
@@ -4278,7 +4278,7 @@
         <v>31</v>
       </c>
       <c r="F46">
-        <f>SUM(G46:R46)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G46">
@@ -4332,7 +4332,7 @@
         <v>20</v>
       </c>
       <c r="F47">
-        <f>SUM(G47:R47)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G47">
@@ -4389,7 +4389,7 @@
         <v>23</v>
       </c>
       <c r="F48">
-        <f>SUM(G48:R48)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G48">
@@ -4443,7 +4443,7 @@
         <v>23</v>
       </c>
       <c r="F49">
-        <f>SUM(G49:R49)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G49">
@@ -4500,7 +4500,7 @@
         <v>101</v>
       </c>
       <c r="F50" s="2">
-        <f>SUM(G50:R50)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G50">
@@ -4557,7 +4557,7 @@
         <v>23</v>
       </c>
       <c r="F51" s="2">
-        <f>SUM(G51:R51)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G51">
@@ -4614,7 +4614,7 @@
         <v>101</v>
       </c>
       <c r="F52">
-        <f>SUM(G52:R52)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G52">
@@ -4671,7 +4671,7 @@
         <v>31</v>
       </c>
       <c r="F53">
-        <f>SUM(G53:R53)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G53">
@@ -4725,7 +4725,7 @@
         <v>23</v>
       </c>
       <c r="F54" s="2">
-        <f>SUM(G54:R54)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G54">
@@ -4782,7 +4782,7 @@
         <v>56</v>
       </c>
       <c r="F55" s="2">
-        <f>SUM(G55:R55)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G55">
@@ -4839,7 +4839,7 @@
         <v>49</v>
       </c>
       <c r="F56">
-        <f>SUM(G56:R56)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G56">
@@ -4890,7 +4890,7 @@
         <v>20</v>
       </c>
       <c r="F57" s="2">
-        <f>SUM(G57:R57)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G57">
@@ -4944,7 +4944,7 @@
         <v>43</v>
       </c>
       <c r="F58">
-        <f>SUM(G58:R58)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G58">
@@ -4998,7 +4998,7 @@
         <v>49</v>
       </c>
       <c r="F59" s="3">
-        <f>SUM(G59:R59)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5019,7 +5019,7 @@
         <v>56</v>
       </c>
       <c r="F60">
-        <f>SUM(G60:R60)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G60">
@@ -5073,7 +5073,7 @@
         <v>20</v>
       </c>
       <c r="F61" s="2">
-        <f>SUM(G61:R61)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G61">
@@ -5130,7 +5130,7 @@
         <v>23</v>
       </c>
       <c r="F62">
-        <f>SUM(G62:R62)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G62">
@@ -5184,7 +5184,7 @@
         <v>101</v>
       </c>
       <c r="F63">
-        <f>SUM(G63:R63)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G63">
@@ -5229,7 +5229,7 @@
         <v>10</v>
       </c>
       <c r="F64">
-        <f>SUM(G64:R64)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="G64">
@@ -5274,7 +5274,7 @@
         <v>28</v>
       </c>
       <c r="F65">
-        <f>SUM(G65:R65)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G65">
@@ -5331,7 +5331,7 @@
         <v>56</v>
       </c>
       <c r="F66">
-        <f>SUM(G66:R66)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G66">
@@ -5385,7 +5385,7 @@
         <v>101</v>
       </c>
       <c r="F67">
-        <f>SUM(G67:R67)</f>
+        <f t="shared" ref="F67:F130" si="2">SUM(G67:R67)</f>
         <v>11</v>
       </c>
       <c r="G67">
@@ -5439,7 +5439,7 @@
         <v>43</v>
       </c>
       <c r="F68">
-        <f>SUM(G68:R68)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G68">
@@ -5493,7 +5493,7 @@
         <v>1</v>
       </c>
       <c r="F69">
-        <f>SUM(G69:R69)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P69">
@@ -5520,7 +5520,7 @@
         <v>28</v>
       </c>
       <c r="F70">
-        <f>SUM(G70:R70)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G70">
@@ -5574,7 +5574,7 @@
         <v>56</v>
       </c>
       <c r="F71">
-        <f>SUM(G71:R71)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G71">
@@ -5628,7 +5628,7 @@
         <v>31</v>
       </c>
       <c r="F72">
-        <f>SUM(G72:R72)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="G72">
@@ -5685,7 +5685,7 @@
         <v>56</v>
       </c>
       <c r="F73">
-        <f>SUM(G73:R73)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="G73">
@@ -5733,7 +5733,7 @@
         <v>23</v>
       </c>
       <c r="F74">
-        <f>SUM(G74:R74)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G74">
@@ -5787,7 +5787,7 @@
         <v>56</v>
       </c>
       <c r="F75">
-        <f>SUM(G75:R75)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G75">
@@ -5841,7 +5841,7 @@
         <v>20</v>
       </c>
       <c r="F76">
-        <f>SUM(G76:R76)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G76">
@@ -5895,7 +5895,7 @@
         <v>49</v>
       </c>
       <c r="F77">
-        <f>SUM(G77:R77)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G77">
@@ -5949,7 +5949,7 @@
         <v>101</v>
       </c>
       <c r="F78">
-        <f>SUM(G78:R78)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G78">
@@ -6003,7 +6003,7 @@
         <v>43</v>
       </c>
       <c r="F79">
-        <f>SUM(G79:R79)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="G79">
@@ -6033,7 +6033,7 @@
         <v>23</v>
       </c>
       <c r="F80">
-        <f>SUM(G80:R80)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G80">
@@ -6087,7 +6087,7 @@
         <v>23</v>
       </c>
       <c r="F81">
-        <f>SUM(G81:R81)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G81">
@@ -6141,7 +6141,7 @@
         <v>49</v>
       </c>
       <c r="F82">
-        <f>SUM(G82:R82)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="G82">
@@ -6198,7 +6198,7 @@
         <v>5</v>
       </c>
       <c r="F83">
-        <f>SUM(G83:R83)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G83">
@@ -6222,7 +6222,7 @@
         <v>28</v>
       </c>
       <c r="F84">
-        <f>SUM(G84:R84)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G84">
@@ -6276,7 +6276,7 @@
         <v>43</v>
       </c>
       <c r="F85">
-        <f>SUM(G85:R85)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G85">
@@ -6330,7 +6330,7 @@
         <v>20</v>
       </c>
       <c r="F86">
-        <f>SUM(G86:R86)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G86">
@@ -6354,7 +6354,7 @@
         <v>28</v>
       </c>
       <c r="F87">
-        <f>SUM(G87:R87)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G87">
@@ -6408,7 +6408,7 @@
         <v>31</v>
       </c>
       <c r="F88">
-        <f>SUM(G88:R88)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G88">
@@ -6462,7 +6462,7 @@
         <v>20</v>
       </c>
       <c r="F89">
-        <f>SUM(G89:R89)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G89">
@@ -6519,7 +6519,7 @@
         <v>23</v>
       </c>
       <c r="F90">
-        <f>SUM(G90:R90)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G90">
@@ -6576,7 +6576,7 @@
         <v>31</v>
       </c>
       <c r="F91">
-        <f>SUM(G91:R91)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="G91">
@@ -6633,7 +6633,7 @@
         <v>31</v>
       </c>
       <c r="F92">
-        <f>SUM(G92:R92)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G92">
@@ -6687,7 +6687,7 @@
         <v>3</v>
       </c>
       <c r="F93">
-        <f>SUM(G93:R93)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="G93">
@@ -6726,7 +6726,7 @@
         <v>101</v>
       </c>
       <c r="F94">
-        <f>SUM(G94:R94)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="G94">
@@ -6774,7 +6774,7 @@
         <v>4</v>
       </c>
       <c r="F95">
-        <f>SUM(G95:R95)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G95">
@@ -6798,7 +6798,7 @@
         <v>28</v>
       </c>
       <c r="F96">
-        <f>SUM(G96:R96)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G96">
@@ -6852,7 +6852,7 @@
         <v>20</v>
       </c>
       <c r="F97">
-        <f>SUM(G97:R97)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G97">
@@ -6906,7 +6906,7 @@
         <v>4</v>
       </c>
       <c r="F98">
-        <f>SUM(G98:R98)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="G98">
@@ -6933,7 +6933,7 @@
         <v>49</v>
       </c>
       <c r="F99">
-        <f>SUM(G99:R99)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="G99">
@@ -6981,7 +6981,7 @@
         <v>46</v>
       </c>
       <c r="F100">
-        <f>SUM(G100:R100)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G100">
@@ -7035,7 +7035,7 @@
         <v>23</v>
       </c>
       <c r="F101">
-        <f>SUM(G101:R101)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G101">
@@ -7059,7 +7059,7 @@
         <v>46</v>
       </c>
       <c r="F102">
-        <f>SUM(G102:R102)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G102">
@@ -7116,7 +7116,7 @@
         <v>23</v>
       </c>
       <c r="F103">
-        <f>SUM(G103:R103)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G103">
@@ -7170,7 +7170,7 @@
         <v>56</v>
       </c>
       <c r="F104">
-        <f>SUM(G104:R104)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G104">
@@ -7224,7 +7224,7 @@
         <v>23</v>
       </c>
       <c r="F105">
-        <f>SUM(G105:R105)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G105">
@@ -7278,7 +7278,7 @@
         <v>28</v>
       </c>
       <c r="F106">
-        <f>SUM(G106:R106)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="G106">
@@ -7335,7 +7335,7 @@
         <v>31</v>
       </c>
       <c r="F107">
-        <f>SUM(G107:R107)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G107">
@@ -7389,7 +7389,7 @@
         <v>46</v>
       </c>
       <c r="F108">
-        <f>SUM(G108:R108)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G108">
@@ -7446,7 +7446,7 @@
         <v>31</v>
       </c>
       <c r="F109">
-        <f>SUM(G109:R109)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G109">
@@ -7500,7 +7500,7 @@
         <v>28</v>
       </c>
       <c r="F110">
-        <f>SUM(G110:R110)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G110">
@@ -7554,7 +7554,7 @@
         <v>20</v>
       </c>
       <c r="F111">
-        <f>SUM(G111:R111)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G111">
@@ -7608,7 +7608,7 @@
         <v>56</v>
       </c>
       <c r="F112">
-        <f>SUM(G112:R112)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G112">
@@ -7632,7 +7632,7 @@
         <v>31</v>
       </c>
       <c r="F113">
-        <f>SUM(G113:R113)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G113">
@@ -7686,7 +7686,7 @@
         <v>38</v>
       </c>
       <c r="F114">
-        <f>SUM(G114:R114)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="G114">
@@ -7743,7 +7743,7 @@
         <v>43</v>
       </c>
       <c r="F115">
-        <f>SUM(G115:R115)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G115">
@@ -7797,7 +7797,7 @@
         <v>49</v>
       </c>
       <c r="F116">
-        <f>SUM(G116:R116)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G116">
@@ -7851,7 +7851,7 @@
         <v>101</v>
       </c>
       <c r="F117">
-        <f>SUM(G117:R117)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="G117">
@@ -7878,7 +7878,7 @@
         <v>23</v>
       </c>
       <c r="F118">
-        <f>SUM(G118:R118)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G118">
@@ -7932,7 +7932,7 @@
         <v>31</v>
       </c>
       <c r="F119">
-        <f>SUM(G119:R119)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G119">
@@ -7986,7 +7986,7 @@
         <v>1</v>
       </c>
       <c r="F120">
-        <f>SUM(G120:R120)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="G120">
@@ -8040,7 +8040,7 @@
         <v>20</v>
       </c>
       <c r="F121">
-        <f>SUM(G121:R121)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G121">
@@ -8097,7 +8097,7 @@
         <v>20</v>
       </c>
       <c r="F122">
-        <f>SUM(G122:R122)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G122">
@@ -8154,7 +8154,7 @@
         <v>46</v>
       </c>
       <c r="F123">
-        <f>SUM(G123:R123)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G123">
@@ -8211,7 +8211,7 @@
         <v>46</v>
       </c>
       <c r="F124">
-        <f>SUM(G124:R124)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="G124">
@@ -8268,7 +8268,7 @@
         <v>20</v>
       </c>
       <c r="F125">
-        <f>SUM(G125:R125)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G125">
@@ -8325,7 +8325,7 @@
         <v>28</v>
       </c>
       <c r="F126">
-        <f>SUM(G126:R126)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G126">
@@ -8379,7 +8379,7 @@
         <v>8</v>
       </c>
       <c r="F127">
-        <f>SUM(G127:R127)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -8400,7 +8400,7 @@
         <v>20</v>
       </c>
       <c r="F128">
-        <f>SUM(G128:R128)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G128">
@@ -8454,7 +8454,7 @@
         <v>56</v>
       </c>
       <c r="F129">
-        <f>SUM(G129:R129)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G129">
@@ -8508,7 +8508,7 @@
         <v>46</v>
       </c>
       <c r="F130">
-        <f>SUM(G130:R130)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G130">
@@ -8565,7 +8565,7 @@
         <v>56</v>
       </c>
       <c r="F131">
-        <f>SUM(G131:R131)</f>
+        <f t="shared" ref="F131:F194" si="3">SUM(G131:R131)</f>
         <v>11</v>
       </c>
       <c r="G131">
@@ -8619,7 +8619,7 @@
         <v>20</v>
       </c>
       <c r="F132">
-        <f>SUM(G132:R132)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -8640,7 +8640,7 @@
         <v>3</v>
       </c>
       <c r="F133">
-        <f>SUM(G133:R133)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G133">
@@ -8682,7 +8682,7 @@
         <v>8</v>
       </c>
       <c r="F134">
-        <f>SUM(G134:R134)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G134">
@@ -8712,7 +8712,7 @@
         <v>101</v>
       </c>
       <c r="F135">
-        <f>SUM(G135:R135)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G135">
@@ -8769,7 +8769,7 @@
         <v>28</v>
       </c>
       <c r="F136">
-        <f>SUM(G136:R136)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="G136">
@@ -8808,7 +8808,7 @@
         <v>23</v>
       </c>
       <c r="F137">
-        <f>SUM(G137:R137)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H137">
@@ -8841,7 +8841,7 @@
         <v>23</v>
       </c>
       <c r="F138">
-        <f>SUM(G138:R138)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G138">
@@ -8895,7 +8895,7 @@
         <v>31</v>
       </c>
       <c r="F139">
-        <f>SUM(G139:R139)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G139">
@@ -8949,7 +8949,7 @@
         <v>101</v>
       </c>
       <c r="F140">
-        <f>SUM(G140:R140)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G140">
@@ -9006,7 +9006,7 @@
         <v>101</v>
       </c>
       <c r="F141">
-        <f>SUM(G141:R141)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G141">
@@ -9063,7 +9063,7 @@
         <v>46</v>
       </c>
       <c r="F142">
-        <f>SUM(G142:R142)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G142">
@@ -9120,7 +9120,7 @@
         <v>28</v>
       </c>
       <c r="F143">
-        <f>SUM(G143:R143)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="G143">
@@ -9177,7 +9177,7 @@
         <v>46</v>
       </c>
       <c r="F144">
-        <f>SUM(G144:R144)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G144">
@@ -9234,7 +9234,7 @@
         <v>43</v>
       </c>
       <c r="F145">
-        <f>SUM(G145:R145)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G145">
@@ -9288,7 +9288,7 @@
         <v>46</v>
       </c>
       <c r="F146">
-        <f>SUM(G146:R146)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G146">
@@ -9342,7 +9342,7 @@
         <v>28</v>
       </c>
       <c r="F147">
-        <f>SUM(G147:R147)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G147">
@@ -9396,7 +9396,7 @@
         <v>56</v>
       </c>
       <c r="F148">
-        <f>SUM(G148:R148)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G148">
@@ -9450,7 +9450,7 @@
         <v>8</v>
       </c>
       <c r="F149">
-        <f>SUM(G149:R149)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="G149">
@@ -9480,7 +9480,7 @@
         <v>46</v>
       </c>
       <c r="F150">
-        <f>SUM(G150:R150)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G150">
@@ -9537,7 +9537,7 @@
         <v>46</v>
       </c>
       <c r="F151">
-        <f>SUM(G151:R151)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G151">
@@ -9591,7 +9591,7 @@
         <v>9</v>
       </c>
       <c r="F152">
-        <f>SUM(G152:R152)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G152">
@@ -9633,7 +9633,7 @@
         <v>28</v>
       </c>
       <c r="F153">
-        <f>SUM(G153:R153)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="G153">
@@ -9690,7 +9690,7 @@
         <v>28</v>
       </c>
       <c r="F154">
-        <f>SUM(G154:R154)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G154">
@@ -9744,7 +9744,7 @@
         <v>20</v>
       </c>
       <c r="F155">
-        <f>SUM(G155:R155)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G155">
@@ -9798,7 +9798,7 @@
         <v>46</v>
       </c>
       <c r="F156">
-        <f>SUM(G156:R156)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G156">
@@ -9852,7 +9852,7 @@
         <v>20</v>
       </c>
       <c r="F157">
-        <f>SUM(G157:R157)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -9873,7 +9873,7 @@
         <v>23</v>
       </c>
       <c r="F158">
-        <f>SUM(G158:R158)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G158">
@@ -9927,7 +9927,7 @@
         <v>23</v>
       </c>
       <c r="F159">
-        <f>SUM(G159:R159)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G159">
@@ -9981,7 +9981,7 @@
         <v>101</v>
       </c>
       <c r="F160">
-        <f>SUM(G160:R160)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G160">
@@ -10038,7 +10038,7 @@
         <v>43</v>
       </c>
       <c r="F161">
-        <f>SUM(G161:R161)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G161">
@@ -10092,7 +10092,7 @@
         <v>43</v>
       </c>
       <c r="F162">
-        <f>SUM(G162:R162)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G162">
@@ -10146,7 +10146,7 @@
         <v>46</v>
       </c>
       <c r="F163">
-        <f>SUM(G163:R163)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="G163">
@@ -10203,7 +10203,7 @@
         <v>56</v>
       </c>
       <c r="F164">
-        <f>SUM(G164:R164)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G164">
@@ -10257,7 +10257,7 @@
         <v>101</v>
       </c>
       <c r="F165">
-        <f>SUM(G165:R165)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G165">
@@ -10314,7 +10314,7 @@
         <v>46</v>
       </c>
       <c r="F166">
-        <f>SUM(G166:R166)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="G166">
@@ -10371,7 +10371,7 @@
         <v>43</v>
       </c>
       <c r="F167">
-        <f>SUM(G167:R167)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G167">
@@ -10425,7 +10425,7 @@
         <v>49</v>
       </c>
       <c r="F168">
-        <f>SUM(G168:R168)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G168">
@@ -10479,7 +10479,7 @@
         <v>101</v>
       </c>
       <c r="F169">
-        <f>SUM(G169:R169)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G169">
@@ -10533,7 +10533,7 @@
         <v>10</v>
       </c>
       <c r="F170">
-        <f>SUM(G170:R170)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G170">
@@ -10557,7 +10557,7 @@
         <v>28</v>
       </c>
       <c r="F171">
-        <f>SUM(G171:R171)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G171">
@@ -10614,7 +10614,7 @@
         <v>28</v>
       </c>
       <c r="F172">
-        <f>SUM(G172:R172)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G172">
@@ -10668,7 +10668,7 @@
         <v>56</v>
       </c>
       <c r="F173">
-        <f>SUM(G173:R173)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G173">
@@ -10722,7 +10722,7 @@
         <v>49</v>
       </c>
       <c r="F174">
-        <f>SUM(G174:R174)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="G174">
@@ -10779,7 +10779,7 @@
         <v>49</v>
       </c>
       <c r="F175">
-        <f>SUM(G175:R175)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="G175">
@@ -10827,7 +10827,7 @@
         <v>46</v>
       </c>
       <c r="F176">
-        <f>SUM(G176:R176)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G176">
@@ -10881,7 +10881,7 @@
         <v>10</v>
       </c>
       <c r="F177">
-        <f>SUM(G177:R177)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="G177">
@@ -10929,7 +10929,7 @@
         <v>56</v>
       </c>
       <c r="F178">
-        <f>SUM(G178:R178)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G178">
@@ -10983,7 +10983,7 @@
         <v>46</v>
       </c>
       <c r="F179">
-        <f>SUM(G179:R179)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="G179">
@@ -11040,7 +11040,7 @@
         <v>101</v>
       </c>
       <c r="F180">
-        <f>SUM(G180:R180)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G180">
@@ -11094,7 +11094,7 @@
         <v>31</v>
       </c>
       <c r="F181">
-        <f>SUM(G181:R181)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="G181">
@@ -11151,7 +11151,7 @@
         <v>23</v>
       </c>
       <c r="F182">
-        <f>SUM(G182:R182)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G182">
@@ -11205,7 +11205,7 @@
         <v>31</v>
       </c>
       <c r="F183">
-        <f>SUM(G183:R183)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G183">
@@ -11259,7 +11259,7 @@
         <v>2</v>
       </c>
       <c r="F184">
-        <f>SUM(G184:R184)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="G184">
@@ -11307,7 +11307,7 @@
         <v>23</v>
       </c>
       <c r="F185">
-        <f>SUM(G185:R185)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G185">
@@ -11361,7 +11361,7 @@
         <v>46</v>
       </c>
       <c r="F186">
-        <f>SUM(G186:R186)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G186">
@@ -11418,7 +11418,7 @@
         <v>101</v>
       </c>
       <c r="F187">
-        <f>SUM(G187:R187)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G187">
@@ -11472,7 +11472,7 @@
         <v>1</v>
       </c>
       <c r="F188">
-        <f>SUM(G188:R188)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P188">
@@ -11499,7 +11499,7 @@
         <v>20</v>
       </c>
       <c r="F189">
-        <f>SUM(G189:R189)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="G189">
@@ -11556,7 +11556,7 @@
         <v>43</v>
       </c>
       <c r="F190">
-        <f>SUM(G190:R190)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G190">
@@ -11610,7 +11610,7 @@
         <v>28</v>
       </c>
       <c r="F191">
-        <f>SUM(G191:R191)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G191">
@@ -11664,7 +11664,7 @@
         <v>7</v>
       </c>
       <c r="F192">
-        <f>SUM(G192:R192)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="G192">
@@ -11709,7 +11709,7 @@
         <v>101</v>
       </c>
       <c r="F193">
-        <f>SUM(G193:R193)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G193">
@@ -11763,7 +11763,7 @@
         <v>43</v>
       </c>
       <c r="F194">
-        <f>SUM(G194:R194)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G194">
@@ -11817,7 +11817,7 @@
         <v>49</v>
       </c>
       <c r="F195">
-        <f>SUM(G195:R195)</f>
+        <f t="shared" ref="F195:F258" si="4">SUM(G195:R195)</f>
         <v>11</v>
       </c>
       <c r="G195">
@@ -11871,7 +11871,7 @@
         <v>28</v>
       </c>
       <c r="F196">
-        <f>SUM(G196:R196)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="G196">
@@ -11925,7 +11925,7 @@
         <v>31</v>
       </c>
       <c r="F197">
-        <f>SUM(G197:R197)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G197">
@@ -11979,7 +11979,7 @@
         <v>10</v>
       </c>
       <c r="F198">
-        <f>SUM(G198:R198)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G198">
@@ -12003,7 +12003,7 @@
         <v>56</v>
       </c>
       <c r="F199">
-        <f>SUM(G199:R199)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G199">
@@ -12057,7 +12057,7 @@
         <v>56</v>
       </c>
       <c r="F200">
-        <f>SUM(G200:R200)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G200">
@@ -12111,7 +12111,7 @@
         <v>38</v>
       </c>
       <c r="F201">
-        <f>SUM(G201:R201)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G201">
@@ -12165,7 +12165,7 @@
         <v>49</v>
       </c>
       <c r="F202">
-        <f>SUM(G202:R202)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -12186,7 +12186,7 @@
         <v>28</v>
       </c>
       <c r="F203">
-        <f>SUM(G203:R203)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="G203">
@@ -12234,7 +12234,7 @@
         <v>23</v>
       </c>
       <c r="F204">
-        <f>SUM(G204:R204)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G204">
@@ -12288,7 +12288,7 @@
         <v>31</v>
       </c>
       <c r="F205">
-        <f>SUM(G205:R205)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G205">
@@ -12342,7 +12342,7 @@
         <v>101</v>
       </c>
       <c r="F206">
-        <f>SUM(G206:R206)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G206">
@@ -12396,7 +12396,7 @@
         <v>20</v>
       </c>
       <c r="F207">
-        <f>SUM(G207:R207)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G207">
@@ -12450,7 +12450,7 @@
         <v>49</v>
       </c>
       <c r="F208">
-        <f>SUM(G208:R208)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G208">
@@ -12504,7 +12504,7 @@
         <v>20</v>
       </c>
       <c r="F209">
-        <f>SUM(G209:R209)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G209">
@@ -12558,7 +12558,7 @@
         <v>23</v>
       </c>
       <c r="F210">
-        <f>SUM(G210:R210)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G210">
@@ -12612,7 +12612,7 @@
         <v>56</v>
       </c>
       <c r="F211">
-        <f>SUM(G211:R211)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G211">
@@ -12666,7 +12666,7 @@
         <v>49</v>
       </c>
       <c r="F212">
-        <f>SUM(G212:R212)</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="G212">
@@ -12723,7 +12723,7 @@
         <v>49</v>
       </c>
       <c r="F213">
-        <f>SUM(G213:R213)</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="G213">
@@ -12780,7 +12780,7 @@
         <v>46</v>
       </c>
       <c r="F214">
-        <f>SUM(G214:R214)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G214">
@@ -12834,7 +12834,7 @@
         <v>8</v>
       </c>
       <c r="F215">
-        <f>SUM(G215:R215)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -12855,7 +12855,7 @@
         <v>28</v>
       </c>
       <c r="F216">
-        <f>SUM(G216:R216)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G216">
@@ -12909,7 +12909,7 @@
         <v>46</v>
       </c>
       <c r="F217">
-        <f>SUM(G217:R217)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G217">
@@ -12963,7 +12963,7 @@
         <v>23</v>
       </c>
       <c r="F218">
-        <f>SUM(G218:R218)</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="G218">
@@ -13020,7 +13020,7 @@
         <v>43</v>
       </c>
       <c r="F219">
-        <f>SUM(G219:R219)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G219">
@@ -13074,7 +13074,7 @@
         <v>28</v>
       </c>
       <c r="F220">
-        <f>SUM(G220:R220)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G220">
@@ -13128,7 +13128,7 @@
         <v>28</v>
       </c>
       <c r="F221">
-        <f>SUM(G221:R221)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G221">
@@ -13182,7 +13182,7 @@
         <v>49</v>
       </c>
       <c r="F222">
-        <f>SUM(G222:R222)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G222">
@@ -13236,7 +13236,7 @@
         <v>101</v>
       </c>
       <c r="F223">
-        <f>SUM(G223:R223)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G223">
@@ -13293,7 +13293,7 @@
         <v>56</v>
       </c>
       <c r="F224">
-        <f>SUM(G224:R224)</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="G224">
@@ -13350,7 +13350,7 @@
         <v>28</v>
       </c>
       <c r="F225">
-        <f>SUM(G225:R225)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K225">
@@ -13374,7 +13374,7 @@
         <v>101</v>
       </c>
       <c r="F226">
-        <f>SUM(G226:R226)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G226">
@@ -13431,7 +13431,7 @@
         <v>43</v>
       </c>
       <c r="F227">
-        <f>SUM(G227:R227)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G227">
@@ -13485,7 +13485,7 @@
         <v>46</v>
       </c>
       <c r="F228">
-        <f>SUM(G228:R228)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="G228">
@@ -13536,7 +13536,7 @@
         <v>43</v>
       </c>
       <c r="F229">
-        <f>SUM(G229:R229)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G229">
@@ -13590,7 +13590,7 @@
         <v>20</v>
       </c>
       <c r="F230">
-        <f>SUM(G230:R230)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G230">
@@ -13644,7 +13644,7 @@
         <v>49</v>
       </c>
       <c r="F231">
-        <f>SUM(G231:R231)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G231">
@@ -13701,7 +13701,7 @@
         <v>38</v>
       </c>
       <c r="F232">
-        <f>SUM(G232:R232)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G232">
@@ -13765,51 +13765,51 @@
         <v>216</v>
       </c>
       <c r="H234">
-        <f t="shared" ref="H234:S234" si="1">SUM(H4:H233)</f>
+        <f t="shared" ref="H234:S234" si="5">SUM(H4:H233)</f>
         <v>208</v>
       </c>
       <c r="I234">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>195</v>
       </c>
       <c r="J234">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>208</v>
       </c>
       <c r="K234">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>190</v>
       </c>
       <c r="L234">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>203</v>
       </c>
       <c r="M234">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>183</v>
       </c>
       <c r="N234">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>198</v>
       </c>
       <c r="O234">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>185</v>
       </c>
       <c r="P234">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>196</v>
       </c>
       <c r="Q234">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>164</v>
       </c>
       <c r="R234">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>54</v>
       </c>
       <c r="S234">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -13880,7 +13880,7 @@
         <v>4</v>
       </c>
       <c r="C239">
-        <f t="shared" ref="C239:C249" si="2">C238+B239</f>
+        <f t="shared" ref="C239:C249" si="6">C238+B239</f>
         <v>22</v>
       </c>
     </row>
@@ -13893,7 +13893,7 @@
         <v>4</v>
       </c>
       <c r="C240">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>26</v>
       </c>
     </row>
@@ -13906,7 +13906,7 @@
         <v>2</v>
       </c>
       <c r="C241">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
     </row>
@@ -13919,7 +13919,7 @@
         <v>2</v>
       </c>
       <c r="C242">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
     </row>
@@ -13932,7 +13932,7 @@
         <v>4</v>
       </c>
       <c r="C243">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>34</v>
       </c>
     </row>
@@ -13945,7 +13945,7 @@
         <v>2</v>
       </c>
       <c r="C244">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>36</v>
       </c>
     </row>
@@ -13958,7 +13958,7 @@
         <v>7</v>
       </c>
       <c r="C245">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>43</v>
       </c>
     </row>
@@ -13971,7 +13971,7 @@
         <v>4</v>
       </c>
       <c r="C246">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>47</v>
       </c>
     </row>
@@ -13984,7 +13984,7 @@
         <v>2</v>
       </c>
       <c r="C247">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>49</v>
       </c>
     </row>
@@ -13997,7 +13997,7 @@
         <v>155</v>
       </c>
       <c r="C248">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>204</v>
       </c>
     </row>
@@ -14010,7 +14010,7 @@
         <v>26</v>
       </c>
       <c r="C249">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>230</v>
       </c>
     </row>

</xml_diff>